<commit_message>
added components spacing configuration
</commit_message>
<xml_diff>
--- a/components.xlsx
+++ b/components.xlsx
@@ -1,46 +1,168 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\文档\0工作资料\国浩工作资料\自有案件\常法——腾讯\99-tools\Attribution_Generator\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A0CEE31-5BEE-4D8E-B33B-699252994464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
+  <si>
+    <t>input_url</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>modified</t>
+  </si>
+  <si>
+    <t>modified_url</t>
+  </si>
+  <si>
+    <t>copyright</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>others_url</t>
+  </si>
+  <si>
+    <t>license</t>
+  </si>
+  <si>
+    <t>package_type</t>
+  </si>
+  <si>
+    <t>repository</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>BSD-3-Clause</t>
+  </si>
+  <si>
+    <t>MIT</t>
+  </si>
+  <si>
+    <t>Copyright (c) 2014-present Matt Zabriskie &amp; Collaborators</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Copyright (c) 2018 Jed Watson</t>
+  </si>
+  <si>
+    <t>Copyright (c) 2018-present, iamkun</t>
+  </si>
+  <si>
+    <t>Copyright (c) 2023 i18next</t>
+  </si>
+  <si>
+    <t>Copyright (c) 2024 i18next</t>
+  </si>
+  <si>
+    <t>Copyright (c) 2018 Copyright 2018 Klaus Hartl, Fagner Brack, GitHub Contributors</t>
+  </si>
+  <si>
+    <t>Copyright © 2011-2012, Paul Vorbach.
+Copyright © 2009, Jeff Mott.</t>
+  </si>
+  <si>
+    <t>Copyright (c) 2024 Vercel, Inc.</t>
+  </si>
+  <si>
+    <t>Copyright (c) Facebook, Inc. and
+its affiliates.</t>
+  </si>
+  <si>
+    <t>Copyright (c) Facebook, Inc. and its affiliates.</t>
+  </si>
+  <si>
+    <t>Copyright (c) 2021-present TDesign</t>
+  </si>
+  <si>
+    <t>Copyright (c) 2019 Paul Henschel</t>
+  </si>
+  <si>
+    <t>axios</t>
+  </si>
+  <si>
+    <t>classnames</t>
+  </si>
+  <si>
+    <t>dayjs</t>
+  </si>
+  <si>
+    <t>i18next</t>
+  </si>
+  <si>
+    <t>i18next-http-backend</t>
+  </si>
+  <si>
+    <t>js-cookie</t>
+  </si>
+  <si>
+    <t>md5</t>
+  </si>
+  <si>
+    <t>next</t>
+  </si>
+  <si>
+    <t>react</t>
+  </si>
+  <si>
+    <t>react-dom</t>
+  </si>
+  <si>
+    <t>react-i18next</t>
+  </si>
+  <si>
+    <t>tdesign-react</t>
+  </si>
+  <si>
+    <t>zustand</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -64,14 +186,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,118 +532,198 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B14"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>input_url</v>
-      </c>
-      <c r="B1" t="str">
-        <v>name</v>
-      </c>
-      <c r="C1" t="str">
-        <v>modified</v>
-      </c>
-      <c r="D1" t="str">
-        <v>modified_url</v>
-      </c>
-      <c r="E1" t="str">
-        <v>copyright</v>
-      </c>
-      <c r="F1" t="str">
-        <v>version</v>
-      </c>
-      <c r="G1" t="str">
-        <v>others_url</v>
-      </c>
-      <c r="H1" t="str">
-        <v>license</v>
-      </c>
-      <c r="I1" t="str">
-        <v>package_type</v>
-      </c>
-      <c r="J1" t="str">
-        <v>repository</v>
-      </c>
-      <c r="K1" t="str">
-        <v>description</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="B2" t="str">
-        <v>transformers</v>
-      </c>
-      <c r="C2" t="str">
+    <row r="1" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="str">
-        <v>Copyright 2018- The Hugging Face team. All rights reserved.</v>
-      </c>
-      <c r="H2" t="str">
-        <v>Apache-2.0</v>
-      </c>
-    </row>
-    <row r="3" xml:space="preserve">
-      <c r="B3" t="str">
-        <v>torch</v>
-      </c>
-      <c r="E3" t="str" xml:space="preserve">
-        <v xml:space="preserve">From PyTorch:_x000d_
-_x000d_
-Copyright (c) 2016-     Facebook, Inc            (Adam Paszke)_x000d_
-Copyright (c) 2014-     Facebook, Inc            (Soumith Chintala)_x000d_
-Copyright (c) 2011-2014 Idiap Research Institute (Ronan Collobert)_x000d_
-Copyright (c) 2012-2014 Deepmind Technologies    (Koray Kavukcuoglu)_x000d_
-Copyright (c) 2011-2012 NEC Laboratories America (Koray Kavukcuoglu)_x000d_
-Copyright (c) 2011-2013 NYU                      (Clement Farabet)_x000d_
-Copyright (c) 2006-2010 NEC Laboratories America (Ronan Collobert, Leon Bottou, Iain Melvin, Jason Weston)_x000d_
-Copyright (c) 2006      Idiap Research Institute (Samy Bengio)_x000d_
-Copyright (c) 2001-2004 Idiap Research Institute (Ronan Collobert, Samy Bengio, Johnny Mariethoz)_x000d_
-_x000d_
-From Caffe2:_x000d_
-_x000d_
-Copyright (c) 2016-present, Facebook Inc. All rights reserved._x000d_
-_x000d_
-All contributions by Facebook:_x000d_
-Copyright (c) 2016 Facebook Inc._x000d_
-_x000d_
-All contributions by Google:_x000d_
-Copyright (c) 2015 Google Inc._x000d_
-All rights reserved._x000d_
-_x000d_
-All contributions by Yangqing Jia:_x000d_
-Copyright (c) 2015 Yangqing Jia_x000d_
-All rights reserved._x000d_
-_x000d_
-All contributions by Kakao Brain:_x000d_
-Copyright 2019-2020 Kakao Brain_x000d_
-_x000d_
-All contributions by Cruise LLC:_x000d_
-Copyright (c) 2022 Cruise LLC._x000d_
-All rights reserved._x000d_
-_x000d_
-All contributions by Arm:_x000d_
-Copyright (c) 2021, 2023-2024 Arm Limited and/or its affiliates_x000d_
-_x000d_
-All contributions from Caffe:_x000d_
-Copyright(c) 2013, 2014, 2015, the respective contributors_x000d_
-All rights reserved._x000d_
-_x000d_
-All other contributions:_x000d_
-Copyright(c) 2015, 2016 the respective contributors_x000d_
-All rights reserved.</v>
-      </c>
-      <c r="H3" t="str">
-        <v>BSD-3-Clause</v>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="165" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K3"/>
+    <ignoredError sqref="A1:K1 A2:A3 I2:K3" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>